<commit_message>
reviewing docs and making minor fixes
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 2/SixGuys_Deliverable_2_SprintBackLog_2.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 2/SixGuys_Deliverable_2_SprintBackLog_2.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCF69E3-B871-4331-9065-7385F8963340}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF1714A-6A28-4F84-AED4-C758338D597B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21900" windowHeight="15180" activeTab="2" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
+    <workbookView xWindow="2055" yWindow="2910" windowWidth="21900" windowHeight="15180" activeTab="2" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2 (2)" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>Player health value and healthbar (can be substituted later for different representation). Plan to add logic to existing enemies to damage player.</t>
+  </si>
+  <si>
+    <t>As a player I want enemies I can engage with so that I can fight them.</t>
+  </si>
+  <si>
+    <t>Ethan Esber 100% Complete</t>
   </si>
 </sst>
 </file>
@@ -333,7 +339,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2013,7 +2019,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,15 +2106,27 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
       <c r="C4" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="20"/>
+        <v>74</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="18">
+        <v>3</v>
+      </c>
+      <c r="F4" s="18">
+        <v>3</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>73</v>
+      </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>